<commit_message>
Continuing to compare past inversions with this one
</commit_message>
<xml_diff>
--- a/paper/tables01.xlsx
+++ b/paper/tables01.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahnesser/Documents/Harvard/Research/TROPOMI_Inversion/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECDDF7A-D34D-9B48-8CBA-BB7E56C640F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFFE98E-0B63-4847-9641-36C9AE20EE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="1160" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{F9FBB28B-7B05-7742-858A-7A42D8F44C3B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{F9FBB28B-7B05-7742-858A-7A42D8F44C3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
   <si>
     <t>Natural</t>
   </si>
@@ -137,9 +138,6 @@
     <t>Oil</t>
   </si>
   <si>
-    <t>Natural gas</t>
-  </si>
-  <si>
     <t xml:space="preserve">Natural </t>
   </si>
   <si>
@@ -158,12 +156,6 @@
     <t>1.4 (1.0 - 1.6)</t>
   </si>
   <si>
-    <t>1.8 (0.81 - 1.9)</t>
-  </si>
-  <si>
-    <t>1.1 (0.76 - 1.6)</t>
-  </si>
-  <si>
     <t>0.69 (0.45 - 0.74)</t>
   </si>
   <si>
@@ -191,12 +183,6 @@
     <t>10.6 (9.2 - 11.8)</t>
   </si>
   <si>
-    <t>4.6 (3.0 - 4.7)</t>
-  </si>
-  <si>
-    <t>9.9 (8.1 - 10.5)</t>
-  </si>
-  <si>
     <t>2.8 (2.4 - 3.5)</t>
   </si>
   <si>
@@ -236,12 +222,6 @@
     <t>2.5 (2.0 - 2.6)</t>
   </si>
   <si>
-    <t>0.84 (0.42 - 0.85)</t>
-  </si>
-  <si>
-    <t>0.42 (0.36 - 0.53)</t>
-  </si>
-  <si>
     <t>0.26 (0.26 - 0.52)</t>
   </si>
   <si>
@@ -267,6 +247,30 @@
   </si>
   <si>
     <t>Gas</t>
+  </si>
+  <si>
+    <t>Hannah xhat (K pos)</t>
+  </si>
+  <si>
+    <t>Hannah xhat std</t>
+  </si>
+  <si>
+    <t>originally 9.4</t>
+  </si>
+  <si>
+    <t>then 6.9</t>
+  </si>
+  <si>
+    <t>2.5 Tg difference</t>
+  </si>
+  <si>
+    <t>3.2 (2.15 - 3.7)</t>
+  </si>
+  <si>
+    <t>14.5 (12.1 -15.1)</t>
+  </si>
+  <si>
+    <t>1.26 (0.84 - 1.37)</t>
   </si>
 </sst>
 </file>
@@ -347,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -372,9 +376,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -390,6 +391,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,15 +746,15 @@
         <v>15.4</v>
       </c>
       <c r="C2" s="4">
-        <f t="shared" ref="C2:E2" si="0">C3+C9</f>
+        <f>C3+C9</f>
         <v>35.5</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" si="0"/>
+        <f>D3+D9</f>
         <v>5.8</v>
       </c>
       <c r="E2" s="4">
-        <f t="shared" si="0"/>
+        <f>E3+E9</f>
         <v>4.5</v>
       </c>
     </row>
@@ -1082,7 +1087,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B27" s="2">
         <v>0.8</v>
@@ -1292,10 +1297,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87290074-0BF1-6644-8DA4-79B4E7E90E5C}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="208" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1305,29 +1313,30 @@
     <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
     <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13" t="s">
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1367,8 +1376,17 @@
       <c r="M2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1376,34 +1394,43 @@
         <v>17.100000000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="17">
-        <f>D13+D4</f>
+        <v>28</v>
+      </c>
+      <c r="D3" s="16">
+        <f>D12+D4</f>
         <v>7.4</v>
       </c>
       <c r="F3">
         <v>36.799999999999997</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="17">
-        <f>H13+H4</f>
+        <v>38</v>
+      </c>
+      <c r="H3" s="16">
+        <f>H12+H4</f>
         <v>30.099999999999998</v>
       </c>
       <c r="J3">
         <v>5.8</v>
       </c>
       <c r="K3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L3" s="17">
-        <f>L13+L4</f>
+        <v>51</v>
+      </c>
+      <c r="L3" s="16">
+        <f>L12+L4</f>
         <v>5.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P3">
+        <v>42.9</v>
+      </c>
+      <c r="Q3">
+        <v>55.64</v>
+      </c>
+      <c r="R3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1411,7 +1438,7 @@
         <v>3.7</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2">
         <v>3.6</v>
@@ -1420,7 +1447,7 @@
         <v>28.7</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H4" s="2">
         <v>26.9</v>
@@ -1429,21 +1456,21 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="L4" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B5">
         <v>1.1000000000000001</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2">
         <v>1.1000000000000001</v>
@@ -1452,422 +1479,412 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="21">
+        <v>40</v>
+      </c>
+      <c r="H5" s="20">
         <v>9.1999999999999993</v>
       </c>
       <c r="J5">
         <v>2.2999999999999998</v>
       </c>
       <c r="K5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="L5" s="2">
         <v>2.4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
-        <v>25</v>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="B6">
-        <v>0.75</v>
-      </c>
-      <c r="C6" t="s">
+        <v>1.55</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F6">
+        <v>9.1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="19">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J6">
+        <v>0.78</v>
+      </c>
+      <c r="K6" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>2.9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="20">
+        <v>2.9</v>
+      </c>
+      <c r="J7">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>0.66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="F8">
+        <v>5.8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="J8">
+        <v>0.77</v>
+      </c>
+      <c r="K8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="J9">
+        <v>0.69</v>
+      </c>
+      <c r="K9" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0.48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="J10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>0.27</v>
+      </c>
+      <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="F6">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="20">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J6">
-        <v>0.44</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="D11" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F11">
+        <v>0.46</v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="J11">
+        <v>0.13</v>
+      </c>
+      <c r="K11" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>13.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="F12">
+        <v>8.6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="J12">
+        <v>0.79</v>
+      </c>
+      <c r="K12" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="F13">
+        <v>7.5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="J13">
+        <v>0.52</v>
+      </c>
+      <c r="K13" t="s">
         <v>59</v>
       </c>
-      <c r="L6" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7">
+      <c r="L13" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2">
         <v>0.8</v>
       </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="F7">
-        <v>6.8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="2">
-        <v>3.4</v>
-      </c>
-      <c r="J7">
-        <v>0.34</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="F14">
+        <v>0.16</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="J14">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K14" t="s">
         <v>60</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>2.9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="21">
-        <v>2.9</v>
-      </c>
-      <c r="J8">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="K8" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>0.66</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="F9">
-        <v>5.8</v>
-      </c>
-      <c r="G9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="J9">
-        <v>0.77</v>
-      </c>
-      <c r="K9" t="s">
-        <v>62</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0.7</v>
-      </c>
-      <c r="G10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="20">
-        <v>0.6</v>
-      </c>
-      <c r="J10">
-        <v>0.69</v>
-      </c>
-      <c r="K10" t="s">
-        <v>63</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0.48</v>
-      </c>
-      <c r="G11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="J11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>0.27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="F12">
-        <v>0.46</v>
-      </c>
-      <c r="G12" t="s">
-        <v>50</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="J12">
-        <v>0.13</v>
-      </c>
-      <c r="K12" t="s">
-        <v>64</v>
-      </c>
-      <c r="L12" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13">
-        <v>13.5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="2">
-        <v>3.8</v>
-      </c>
-      <c r="F13">
-        <v>8.6</v>
-      </c>
-      <c r="G13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" s="2">
-        <v>3.2</v>
-      </c>
-      <c r="J13">
-        <v>0.79</v>
-      </c>
-      <c r="K13" t="s">
-        <v>65</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="2">
-        <v>2.6</v>
-      </c>
-      <c r="F14">
-        <v>7.5</v>
-      </c>
-      <c r="G14" t="s">
-        <v>52</v>
-      </c>
-      <c r="H14" s="2">
-        <v>2.1</v>
-      </c>
-      <c r="J14">
-        <v>0.52</v>
-      </c>
-      <c r="K14" t="s">
-        <v>66</v>
       </c>
       <c r="L14" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
-        <v>8</v>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="B15">
-        <v>1.1000000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" s="2">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="F15">
-        <v>0.16</v>
+        <v>0.59</v>
       </c>
       <c r="G15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H15" s="2">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="J15">
-        <v>0.14000000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="K15" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="L15" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="2">
         <v>0.3</v>
       </c>
-      <c r="F16">
-        <v>0.59</v>
-      </c>
-      <c r="G16" t="s">
-        <v>54</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="J16">
-        <v>0.13</v>
+      <c r="J16" t="s">
+        <v>29</v>
       </c>
       <c r="K16" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="L16" s="2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="G17" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="J17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K17" t="s">
-        <v>30</v>
-      </c>
-      <c r="L17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H18" s="2"/>
-      <c r="L18" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="16"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
@@ -1968,17 +1985,10 @@
       <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="19"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>